<commit_message>
working on the csv
</commit_message>
<xml_diff>
--- a/tables/Literaturrecherche.xlsx
+++ b/tables/Literaturrecherche.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Cluster" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$K$149</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$O$152</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$O$152</definedName>
   </definedNames>
   <calcPr/>
   <extLst>
@@ -22,9 +22,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="469">
-  <si>
-    <t>ID</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="472">
+  <si>
+    <t>Id</t>
   </si>
   <si>
     <t>Autor</t>
@@ -66,7 +66,7 @@
     <t>Dokumentation</t>
   </si>
   <si>
-    <t xml:space="preserve">Anzahl Zitationen</t>
+    <t>Zitationen</t>
   </si>
   <si>
     <t xml:space="preserve">P. W. C. Prasad, A. Alsadoon, A. Beg, A. Chan </t>
@@ -90,9 +90,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>0,1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Z. Radivojevic, Z. Stanisavljevic, M. Punt</t>
   </si>
   <si>
@@ -144,7 +141,7 @@
     <t xml:space="preserve">Applying a Constructivist and Collaborative Methodological Approach in Engineering Education</t>
   </si>
   <si>
-    <t xml:space="preserve">Computers &amp; Education</t>
+    <t xml:space="preserve">Computers and Education</t>
   </si>
   <si>
     <t>Superskalarität</t>
@@ -207,7 +204,7 @@
     <t xml:space="preserve">S. N. Soares, F. R. Wagner</t>
   </si>
   <si>
-    <t xml:space="preserve">T&amp;D-Bench-Innovative Combined Support for Education and Research in Computer Architecture and Embedded Systems</t>
+    <t xml:space="preserve">T\&amp;D-Bench-Innovative Combined Support for Education and Research in Computer Architecture and Embedded Systems</t>
   </si>
   <si>
     <t>ADL</t>
@@ -249,7 +246,7 @@
     <t xml:space="preserve">Software Package for an Educational Computer System</t>
   </si>
   <si>
-    <t xml:space="preserve">International Journal of Electrical Engineering &amp; Education</t>
+    <t xml:space="preserve">International Journal of Electrical Engineering an Education</t>
   </si>
   <si>
     <t xml:space="preserve">C. Yehezkel, W. Yurcik, M. Pearson, D. Armstrong</t>
@@ -327,6 +324,9 @@
     <t xml:space="preserve">WASP: A Web-Based Simulator for an Educational Pipelined Processor</t>
   </si>
   <si>
+    <t xml:space="preserve">International Journal of Electrical Engineering and Education</t>
+  </si>
+  <si>
     <t xml:space="preserve">P. Paczula, R. Tutajewicz, R. Brzeski, H. Zghidi, A. Momot, E. Pluciennik, A. Duszenki, S. Kozielski, D. Mrozek</t>
   </si>
   <si>
@@ -435,7 +435,7 @@
     <t xml:space="preserve">SP-1: Design and Simulation of 4-bit Simple CPU on Logisim for Computer Architecture Education</t>
   </si>
   <si>
-    <t xml:space="preserve">International Conference on Electrical, Computer &amp; Telecommunication Engineering</t>
+    <t xml:space="preserve">International Conference on Electrical, Computer and Telecommunication Engineering</t>
   </si>
   <si>
     <t xml:space="preserve">A. Mosallaei, K. E. Isaacs, Y. Sun</t>
@@ -537,7 +537,7 @@
     <t xml:space="preserve">A lightweight instruction-set simulator for teaching of dynamic instruction scheduling</t>
   </si>
   <si>
-    <t xml:space="preserve">International Conference on Computer Science &amp; Education</t>
+    <t xml:space="preserve">International Conference on Computer Science and Education</t>
   </si>
   <si>
     <t xml:space="preserve">R. Desikan, D. Burger, S. W. Keckler</t>
@@ -684,7 +684,7 @@
     <t xml:space="preserve">J. Mendes, Rajesh C. Panicker</t>
   </si>
   <si>
-    <t xml:space="preserve">RISCALAR: A Cycle-Approximate, Parametrisable RISC-V Microarchitecture Explorer &amp; Simulator</t>
+    <t xml:space="preserve">RISCALAR: A Cycle-Approximate, Parametrisable RISC-V Microarchitecture Explorer \&amp; Simulator</t>
   </si>
   <si>
     <t xml:space="preserve">IEEE International Symposium on Circuits and Systems </t>
@@ -798,6 +798,9 @@
     <t>Book</t>
   </si>
   <si>
+    <t xml:space="preserve">Packt Publishing</t>
+  </si>
+  <si>
     <t xml:space="preserve">M. Yang</t>
   </si>
   <si>
@@ -1050,7 +1053,7 @@
     <t xml:space="preserve">Cloud Computing</t>
   </si>
   <si>
-    <t>4</t>
+    <t>3</t>
   </si>
   <si>
     <t xml:space="preserve">Y. Li, Y. Bao, G. Wang, X. Mei, P. Vaid, A. Ghosh, A. Jog, D. Bunander, A. Joshi, Y. Sun</t>
@@ -1275,6 +1278,9 @@
     <t xml:space="preserve">Using EDUCache simulator for the computer architecture and organization course</t>
   </si>
   <si>
+    <t xml:space="preserve">International Journal of Engineering Pedagogy</t>
+  </si>
+  <si>
     <t xml:space="preserve">A. M. DeNardo, A. S. Pyzdrowski</t>
   </si>
   <si>
@@ -1398,6 +1404,9 @@
     <t xml:space="preserve">keine Information</t>
   </si>
   <si>
+    <t xml:space="preserve">on- und offline</t>
+  </si>
+  <si>
     <t>kostenlos</t>
   </si>
   <si>
@@ -1413,22 +1422,22 @@
     <t>Thema</t>
   </si>
   <si>
-    <t xml:space="preserve">Grundlagen &amp; Theorien</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prozessoren &amp; Architekturen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speicher &amp; Performance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hardware &amp; Logik</t>
+    <t xml:space="preserve">Grundlagen und Theorien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prozessoren und Architekturen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speicher und Performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hardware und Logik</t>
   </si>
   <si>
     <t>Programmierung</t>
   </si>
   <si>
-    <t xml:space="preserve">Systeme &amp; Anwendungen</t>
+    <t xml:space="preserve">Systeme und Anwendungen</t>
   </si>
 </sst>
 </file>
@@ -2134,8 +2143,7 @@
     <col bestFit="1" customWidth="1" min="4" max="4" style="1" width="7.140625"/>
     <col customWidth="1" min="5" max="5" style="1" width="16.351600000000001"/>
     <col customWidth="1" min="6" max="6" style="1" width="35.8515625"/>
-    <col customWidth="1" min="7" max="7" style="1" width="16.351600000000001"/>
-    <col customWidth="1" min="8" max="8" style="1" width="16.351600000000001"/>
+    <col customWidth="1" min="7" max="8" style="1" width="16.351600000000001"/>
     <col customWidth="1" min="9" max="9" style="2" width="16.351600000000001"/>
     <col customWidth="1" min="10" max="10" style="2" width="15.7109375"/>
     <col customWidth="1" min="11" max="15" style="2" width="16.351600000000001"/>
@@ -2224,8 +2232,8 @@
       <c r="K2" s="2">
         <v>1</v>
       </c>
-      <c r="L2" s="8" t="s">
-        <v>22</v>
+      <c r="L2" s="8">
+        <v>3</v>
       </c>
       <c r="M2" s="2">
         <v>0</v>
@@ -2242,10 +2250,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="D3" s="1">
         <v>2018</v>
@@ -2257,11 +2265,11 @@
         <v>18</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H3" s="1" t="str">
         <f>VLOOKUP(G3,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>20</v>
@@ -2290,10 +2298,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="D4" s="1">
         <v>2024</v>
@@ -2302,14 +2310,14 @@
         <v>17</v>
       </c>
       <c r="F4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="H4" s="1" t="str">
         <f>VLOOKUP(G4,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>20</v>
@@ -2338,10 +2346,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="D5" s="1">
         <v>2024</v>
@@ -2350,14 +2358,14 @@
         <v>17</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="H5" s="1" t="str">
         <f>VLOOKUP(G5,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>20</v>
@@ -2386,10 +2394,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>35</v>
       </c>
       <c r="D6" s="1">
         <v>2022</v>
@@ -2398,14 +2406,14 @@
         <v>17</v>
       </c>
       <c r="F6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="H6" s="1" t="str">
         <f>VLOOKUP(G6,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Hardware &amp; Logik</v>
+        <v xml:space="preserve">Hardware und Logik</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>20</v>
@@ -2434,10 +2442,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>39</v>
       </c>
       <c r="D7" s="1">
         <v>2007</v>
@@ -2446,14 +2454,14 @@
         <v>17</v>
       </c>
       <c r="F7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>41</v>
       </c>
       <c r="H7" s="1" t="str">
         <f>VLOOKUP(G7,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>20</v>
@@ -2464,8 +2472,8 @@
       <c r="K7" s="2">
         <v>1</v>
       </c>
-      <c r="L7" s="8" t="s">
-        <v>22</v>
+      <c r="L7" s="8">
+        <v>3</v>
       </c>
       <c r="M7" s="2">
         <v>0</v>
@@ -2482,10 +2490,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="D8" s="1">
         <v>2020</v>
@@ -2494,14 +2502,14 @@
         <v>17</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H8" s="1" t="str">
         <f>VLOOKUP(G8,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Hardware &amp; Logik</v>
+        <v xml:space="preserve">Hardware und Logik</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>20</v>
@@ -2530,10 +2538,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="D9" s="1">
         <v>2012</v>
@@ -2542,14 +2550,14 @@
         <v>17</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" s="1" t="str">
         <f>VLOOKUP(G9,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>20</v>
@@ -2560,8 +2568,8 @@
       <c r="K9" s="2">
         <v>1</v>
       </c>
-      <c r="L9" s="8" t="s">
-        <v>22</v>
+      <c r="L9" s="8">
+        <v>3</v>
       </c>
       <c r="M9" s="2">
         <v>0</v>
@@ -2578,10 +2586,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="D10" s="1">
         <v>2015</v>
@@ -2593,11 +2601,11 @@
         <v>18</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H10" s="1" t="str">
         <f>VLOOKUP(G10,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>20</v>
@@ -2626,10 +2634,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="D11" s="1">
         <v>2012</v>
@@ -2638,14 +2646,14 @@
         <v>17</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H11" s="1" t="str">
         <f>VLOOKUP(G11,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>20</v>
@@ -2674,10 +2682,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="D12" s="1">
         <v>2015</v>
@@ -2722,10 +2730,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="D13" s="1">
         <v>2010</v>
@@ -2734,14 +2742,14 @@
         <v>17</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H13" s="1" t="str">
         <f>VLOOKUP(G13,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>20</v>
@@ -2752,8 +2760,8 @@
       <c r="K13" s="2">
         <v>1</v>
       </c>
-      <c r="L13" s="8" t="s">
-        <v>22</v>
+      <c r="L13" s="8">
+        <v>3</v>
       </c>
       <c r="M13" s="2">
         <v>0</v>
@@ -2770,10 +2778,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="D14" s="1">
         <v>2005</v>
@@ -2782,14 +2790,14 @@
         <v>17</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H14" s="1" t="str">
         <f>VLOOKUP(G14,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Grundlagen &amp; Theorien</v>
+        <v xml:space="preserve">Grundlagen und Theorien</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>20</v>
@@ -2818,10 +2826,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="D15" s="1">
         <v>2011</v>
@@ -2830,14 +2838,14 @@
         <v>17</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H15" s="1" t="str">
         <f>VLOOKUP(G15,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Grundlagen &amp; Theorien</v>
+        <v xml:space="preserve">Grundlagen und Theorien</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>20</v>
@@ -2866,10 +2874,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>64</v>
       </c>
       <c r="D16" s="1">
         <v>2015</v>
@@ -2881,11 +2889,11 @@
         <v>18</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H16" s="1" t="str">
         <f>VLOOKUP(G16,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>20</v>
@@ -2914,10 +2922,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="D17" s="1">
         <v>2011</v>
@@ -2929,11 +2937,11 @@
         <v>18</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H17" s="1" t="str">
         <f>VLOOKUP(G17,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Speicher &amp; Performance</v>
+        <v xml:space="preserve">Speicher und Performance</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>20</v>
@@ -2962,26 +2970,26 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="D18" s="1">
         <v>2018</v>
       </c>
       <c r="E18" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>71</v>
-      </c>
       <c r="G18" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H18" s="1" t="str">
         <f>VLOOKUP(G18,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I18" s="7" t="s">
         <v>20</v>
@@ -3010,10 +3018,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D19" s="1">
         <v>2007</v>
@@ -3022,14 +3030,14 @@
         <v>17</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H19" s="1" t="str">
         <f>VLOOKUP(G19,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I19" s="7" t="s">
         <v>20</v>
@@ -3040,8 +3048,8 @@
       <c r="K19" s="2">
         <v>1</v>
       </c>
-      <c r="L19" s="8" t="s">
-        <v>22</v>
+      <c r="L19" s="8">
+        <v>3</v>
       </c>
       <c r="M19" s="2">
         <v>0</v>
@@ -3058,10 +3066,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>74</v>
       </c>
       <c r="D20" s="1">
         <v>2003</v>
@@ -3070,14 +3078,14 @@
         <v>17</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H20" s="1" t="str">
         <f>VLOOKUP(G20,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>20</v>
@@ -3106,10 +3114,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>77</v>
       </c>
       <c r="D21" s="1">
         <v>2001</v>
@@ -3118,14 +3126,14 @@
         <v>17</v>
       </c>
       <c r="F21" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="H21" s="1" t="str">
         <f>VLOOKUP(G21,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I21" s="7" t="s">
         <v>20</v>
@@ -3154,10 +3162,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>81</v>
       </c>
       <c r="D22" s="1">
         <v>2003</v>
@@ -3166,7 +3174,7 @@
         <v>17</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>19</v>
@@ -3202,10 +3210,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="D23" s="1">
         <v>2001</v>
@@ -3214,14 +3222,14 @@
         <v>17</v>
       </c>
       <c r="F23" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="H23" s="1" t="str">
         <f>VLOOKUP(G23,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I23" s="7" t="s">
         <v>20</v>
@@ -3250,10 +3258,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>85</v>
       </c>
       <c r="D24" s="1">
         <v>2002</v>
@@ -3262,7 +3270,7 @@
         <v>17</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>19</v>
@@ -3298,10 +3306,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>87</v>
       </c>
       <c r="D25" s="1">
         <v>2002</v>
@@ -3310,14 +3318,14 @@
         <v>17</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H25" s="1" t="str">
         <f>VLOOKUP(G25,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I25" s="7" t="s">
         <v>20</v>
@@ -3346,10 +3354,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>88</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>89</v>
       </c>
       <c r="D26" s="1">
         <v>2001</v>
@@ -3358,7 +3366,7 @@
         <v>17</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>19</v>
@@ -3394,10 +3402,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>91</v>
       </c>
       <c r="D27" s="1">
         <v>2001</v>
@@ -3406,14 +3414,14 @@
         <v>17</v>
       </c>
       <c r="F27" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G27" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="H27" s="1" t="str">
         <f>VLOOKUP(G27,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I27" s="7" t="s">
         <v>20</v>
@@ -3442,10 +3450,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="D28" s="1">
         <v>2018</v>
@@ -3457,11 +3465,11 @@
         <v>18</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H28" s="1" t="str">
         <f>VLOOKUP(G28,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I28" s="7" t="s">
         <v>20</v>
@@ -3490,10 +3498,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>96</v>
       </c>
       <c r="D29" s="1">
         <v>2001</v>
@@ -3502,14 +3510,14 @@
         <v>17</v>
       </c>
       <c r="F29" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G29" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>98</v>
       </c>
       <c r="H29" s="1" t="str">
         <f>VLOOKUP(G29,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Speicher &amp; Performance</v>
+        <v xml:space="preserve">Speicher und Performance</v>
       </c>
       <c r="I29" s="7" t="s">
         <v>20</v>
@@ -3538,10 +3546,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>100</v>
       </c>
       <c r="D30" s="1">
         <v>2007</v>
@@ -3550,14 +3558,14 @@
         <v>17</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H30" s="1" t="str">
         <f>VLOOKUP(G30,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I30" s="7" t="s">
         <v>20</v>
@@ -3601,11 +3609,11 @@
         <v>104</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H31" s="1" t="str">
         <f>VLOOKUP(G31,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I31" s="7" t="s">
         <v>20</v>
@@ -3649,11 +3657,11 @@
         <v>107</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H32" s="1" t="str">
         <f>VLOOKUP(G32,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I32" s="7" t="s">
         <v>20</v>
@@ -3697,11 +3705,11 @@
         <v>110</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H33" s="1" t="str">
         <f>VLOOKUP(G33,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I33" s="7" t="s">
         <v>20</v>
@@ -3745,11 +3753,11 @@
         <v>113</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H34" s="1" t="str">
         <f>VLOOKUP(G34,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I34" s="7" t="s">
         <v>20</v>
@@ -3760,8 +3768,8 @@
       <c r="K34" s="2">
         <v>1</v>
       </c>
-      <c r="L34" s="8" t="s">
-        <v>22</v>
+      <c r="L34" s="8">
+        <v>3</v>
       </c>
       <c r="M34" s="2">
         <v>0</v>
@@ -3793,11 +3801,11 @@
         <v>116</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H35" s="1" t="str">
         <f>VLOOKUP(G35,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I35" s="7" t="s">
         <v>20</v>
@@ -3808,8 +3816,8 @@
       <c r="K35" s="2">
         <v>1</v>
       </c>
-      <c r="L35" s="2" t="s">
-        <v>22</v>
+      <c r="L35" s="2">
+        <v>3</v>
       </c>
       <c r="M35" s="2">
         <v>0</v>
@@ -3841,11 +3849,11 @@
         <v>119</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H36" s="1" t="str">
         <f>VLOOKUP(G36,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Speicher &amp; Performance</v>
+        <v xml:space="preserve">Speicher und Performance</v>
       </c>
       <c r="I36" s="7" t="s">
         <v>20</v>
@@ -3889,11 +3897,11 @@
         <v>122</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H37" s="1" t="str">
         <f>VLOOKUP(G37,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I37" s="7" t="s">
         <v>20</v>
@@ -3937,11 +3945,11 @@
         <v>125</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H38" s="1" t="str">
         <f>VLOOKUP(G38,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I38" s="7" t="s">
         <v>20</v>
@@ -3989,7 +3997,7 @@
       </c>
       <c r="H39" s="1" t="str">
         <f>VLOOKUP(G39,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Grundlagen &amp; Theorien</v>
+        <v xml:space="preserve">Grundlagen und Theorien</v>
       </c>
       <c r="I39" s="7" t="s">
         <v>20</v>
@@ -4033,11 +4041,11 @@
         <v>131</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H40" s="1" t="str">
         <f>VLOOKUP(G40,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I40" s="7" t="s">
         <v>20</v>
@@ -4081,11 +4089,11 @@
         <v>134</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H41" s="1" t="str">
         <f>VLOOKUP(G41,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I41" s="7" t="s">
         <v>20</v>
@@ -4129,11 +4137,11 @@
         <v>137</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H42" s="1" t="str">
         <f>VLOOKUP(G42,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I42" s="7" t="s">
         <v>20</v>
@@ -4229,7 +4237,7 @@
       </c>
       <c r="H44" s="1" t="str">
         <f>VLOOKUP(G44,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Speicher &amp; Performance</v>
+        <v xml:space="preserve">Speicher und Performance</v>
       </c>
       <c r="I44" s="7" t="s">
         <v>20</v>
@@ -4273,11 +4281,11 @@
         <v>148</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H45" s="1" t="str">
         <f>VLOOKUP(G45,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I45" s="7" t="s">
         <v>20</v>
@@ -4321,11 +4329,11 @@
         <v>122</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H46" s="1" t="str">
         <f>VLOOKUP(G46,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I46" s="7" t="s">
         <v>20</v>
@@ -4366,14 +4374,14 @@
         <v>17</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>153</v>
       </c>
       <c r="H47" s="1" t="str">
         <f>VLOOKUP(G47,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I47" s="7" t="s">
         <v>20</v>
@@ -4414,14 +4422,14 @@
         <v>17</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>153</v>
       </c>
       <c r="H48" s="1" t="str">
         <f>VLOOKUP(G48,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I48" s="7" t="s">
         <v>20</v>
@@ -4433,7 +4441,7 @@
         <v>1</v>
       </c>
       <c r="L48" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M48" s="2">
         <v>2</v>
@@ -4561,11 +4569,11 @@
         <v>162</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H51" s="1" t="str">
         <f>VLOOKUP(G51,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Speicher &amp; Performance</v>
+        <v xml:space="preserve">Speicher und Performance</v>
       </c>
       <c r="I51" s="7" t="s">
         <v>20</v>
@@ -4609,11 +4617,11 @@
         <v>165</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H52" s="1" t="str">
         <f>VLOOKUP(G52,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I52" s="7" t="s">
         <v>20</v>
@@ -4624,8 +4632,8 @@
       <c r="K52" s="2">
         <v>1</v>
       </c>
-      <c r="L52" s="8" t="s">
-        <v>22</v>
+      <c r="L52" s="8">
+        <v>3</v>
       </c>
       <c r="M52" s="2">
         <v>0</v>
@@ -4657,11 +4665,11 @@
         <v>168</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H53" s="1" t="str">
         <f>VLOOKUP(G53,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I53" s="7" t="s">
         <v>20</v>
@@ -4705,11 +4713,11 @@
         <v>171</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H54" s="1" t="str">
         <f>VLOOKUP(G54,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I54" s="7" t="s">
         <v>20</v>
@@ -4753,11 +4761,11 @@
         <v>144</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H55" s="1" t="str">
         <f>VLOOKUP(G55,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I55" s="7" t="s">
         <v>20</v>
@@ -4798,14 +4806,14 @@
         <v>17</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H56" s="1" t="str">
         <f>VLOOKUP(G56,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I56" s="7" t="s">
         <v>20</v>
@@ -4816,8 +4824,8 @@
       <c r="K56" s="2">
         <v>1</v>
       </c>
-      <c r="L56" s="8" t="s">
-        <v>22</v>
+      <c r="L56" s="8">
+        <v>3</v>
       </c>
       <c r="M56" s="2">
         <v>0</v>
@@ -4853,7 +4861,7 @@
       </c>
       <c r="H57" s="1" t="str">
         <f>VLOOKUP(G57,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Hardware &amp; Logik</v>
+        <v xml:space="preserve">Hardware und Logik</v>
       </c>
       <c r="I57" s="7" t="s">
         <v>20</v>
@@ -4894,7 +4902,7 @@
         <v>17</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G58" s="6" t="s">
         <v>19</v>
@@ -4949,7 +4957,7 @@
       </c>
       <c r="H59" s="1" t="str">
         <f>VLOOKUP(G59,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Grundlagen &amp; Theorien</v>
+        <v xml:space="preserve">Grundlagen und Theorien</v>
       </c>
       <c r="I59" s="7" t="s">
         <v>20</v>
@@ -4993,11 +5001,11 @@
         <v>188</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H60" s="1" t="str">
         <f>VLOOKUP(G60,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I60" s="7" t="s">
         <v>20</v>
@@ -5008,8 +5016,8 @@
       <c r="K60" s="2">
         <v>1</v>
       </c>
-      <c r="L60" s="8" t="s">
-        <v>22</v>
+      <c r="L60" s="8">
+        <v>3</v>
       </c>
       <c r="M60" s="2">
         <v>0</v>
@@ -5041,11 +5049,11 @@
         <v>144</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H61" s="1" t="str">
         <f>VLOOKUP(G61,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I61" s="7" t="s">
         <v>20</v>
@@ -5089,11 +5097,11 @@
         <v>122</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H62" s="1" t="str">
         <f>VLOOKUP(G62,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I62" s="7" t="s">
         <v>20</v>
@@ -5104,8 +5112,8 @@
       <c r="K62" s="2">
         <v>1</v>
       </c>
-      <c r="L62" s="2" t="s">
-        <v>22</v>
+      <c r="L62" s="2">
+        <v>3</v>
       </c>
       <c r="M62" s="2">
         <v>0</v>
@@ -5141,7 +5149,7 @@
       </c>
       <c r="H63" s="1" t="str">
         <f>VLOOKUP(G63,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Grundlagen &amp; Theorien</v>
+        <v xml:space="preserve">Grundlagen und Theorien</v>
       </c>
       <c r="I63" s="7" t="s">
         <v>21</v>
@@ -5189,7 +5197,7 @@
       </c>
       <c r="H64" s="1" t="str">
         <f>VLOOKUP(G64,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Systeme &amp; Anwendungen</v>
+        <v xml:space="preserve">Systeme und Anwendungen</v>
       </c>
       <c r="I64" s="7" t="s">
         <v>20</v>
@@ -5237,7 +5245,7 @@
       </c>
       <c r="H65" s="1" t="str">
         <f>VLOOKUP(G65,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Speicher &amp; Performance</v>
+        <v xml:space="preserve">Speicher und Performance</v>
       </c>
       <c r="I65" s="7" t="s">
         <v>20</v>
@@ -5285,7 +5293,7 @@
       </c>
       <c r="H66" s="1" t="str">
         <f>VLOOKUP(G66,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Hardware &amp; Logik</v>
+        <v xml:space="preserve">Hardware und Logik</v>
       </c>
       <c r="I66" s="7" t="s">
         <v>20</v>
@@ -5377,11 +5385,11 @@
         <v>213</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H68" s="1" t="str">
         <f>VLOOKUP(G68,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I68" s="7" t="s">
         <v>20</v>
@@ -5422,14 +5430,14 @@
         <v>17</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H69" s="1" t="str">
         <f>VLOOKUP(G69,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I69" s="7" t="s">
         <v>20</v>
@@ -5473,11 +5481,11 @@
         <v>218</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H70" s="1" t="str">
         <f>VLOOKUP(G70,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I70" s="7" t="s">
         <v>20</v>
@@ -5521,11 +5529,11 @@
         <v>221</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H71" s="1" t="str">
         <f>VLOOKUP(G71,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I71" s="7" t="s">
         <v>20</v>
@@ -5573,7 +5581,7 @@
       </c>
       <c r="H72" s="1" t="str">
         <f>VLOOKUP(G72,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Hardware &amp; Logik</v>
+        <v xml:space="preserve">Hardware und Logik</v>
       </c>
       <c r="I72" s="7" t="s">
         <v>20</v>
@@ -5617,11 +5625,11 @@
         <v>228</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H73" s="1" t="str">
         <f>VLOOKUP(G73,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I73" s="7" t="s">
         <v>20</v>
@@ -5665,11 +5673,11 @@
         <v>178</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H74" s="1" t="str">
         <f>VLOOKUP(G74,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Speicher &amp; Performance</v>
+        <v xml:space="preserve">Speicher und Performance</v>
       </c>
       <c r="I74" s="7" t="s">
         <v>20</v>
@@ -5717,7 +5725,7 @@
       </c>
       <c r="H75" s="1" t="str">
         <f>VLOOKUP(G75,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Hardware &amp; Logik</v>
+        <v xml:space="preserve">Hardware und Logik</v>
       </c>
       <c r="I75" s="7" t="s">
         <v>20</v>
@@ -5809,11 +5817,11 @@
         <v>134</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H77" s="1" t="str">
         <f>VLOOKUP(G77,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Speicher &amp; Performance</v>
+        <v xml:space="preserve">Speicher und Performance</v>
       </c>
       <c r="I77" s="7" t="s">
         <v>20</v>
@@ -5857,11 +5865,11 @@
         <v>241</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H78" s="1" t="str">
         <f>VLOOKUP(G78,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I78" s="7" t="s">
         <v>20</v>
@@ -5953,11 +5961,11 @@
         <v>171</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H80" s="1" t="str">
         <f>VLOOKUP(G80,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I80" s="7" t="s">
         <v>20</v>
@@ -6001,11 +6009,11 @@
         <v>249</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H81" s="1" t="str">
         <f>VLOOKUP(G81,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I81" s="7" t="s">
         <v>20</v>
@@ -6049,11 +6057,11 @@
         <v>178</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H82" s="1" t="str">
         <f>VLOOKUP(G82,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Speicher &amp; Performance</v>
+        <v xml:space="preserve">Speicher und Performance</v>
       </c>
       <c r="I82" s="7" t="s">
         <v>20</v>
@@ -6101,7 +6109,7 @@
       </c>
       <c r="H83" s="1" t="str">
         <f>VLOOKUP(G83,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Grundlagen &amp; Theorien</v>
+        <v xml:space="preserve">Grundlagen und Theorien</v>
       </c>
       <c r="I83" s="7" t="s">
         <v>20</v>
@@ -6141,13 +6149,15 @@
       <c r="E84" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="F84" s="1"/>
+      <c r="F84" s="1" t="s">
+        <v>258</v>
+      </c>
       <c r="G84" s="6" t="s">
         <v>196</v>
       </c>
       <c r="H84" s="1" t="str">
         <f>VLOOKUP(G84,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Grundlagen &amp; Theorien</v>
+        <v xml:space="preserve">Grundlagen und Theorien</v>
       </c>
       <c r="I84" s="7" t="s">
         <v>20</v>
@@ -6176,10 +6186,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D85" s="1">
         <v>2021</v>
@@ -6188,14 +6198,14 @@
         <v>103</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H85" s="1" t="str">
         <f>VLOOKUP(G85,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Systeme &amp; Anwendungen</v>
+        <v xml:space="preserve">Systeme und Anwendungen</v>
       </c>
       <c r="I85" s="7" t="s">
         <v>20</v>
@@ -6224,10 +6234,10 @@
         <v>85</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D86" s="1">
         <v>2019</v>
@@ -6236,7 +6246,7 @@
         <v>103</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G86" s="6" t="s">
         <v>210</v>
@@ -6272,10 +6282,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D87" s="1">
         <v>2024</v>
@@ -6284,14 +6294,14 @@
         <v>103</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G87" s="6" t="s">
         <v>179</v>
       </c>
       <c r="H87" s="1" t="str">
         <f>VLOOKUP(G87,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Hardware &amp; Logik</v>
+        <v xml:space="preserve">Hardware und Logik</v>
       </c>
       <c r="I87" s="7" t="s">
         <v>20</v>
@@ -6320,10 +6330,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D88" s="1">
         <v>2022</v>
@@ -6332,14 +6342,14 @@
         <v>103</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H88" s="1" t="str">
         <f>VLOOKUP(G88,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Speicher &amp; Performance</v>
+        <v xml:space="preserve">Speicher und Performance</v>
       </c>
       <c r="I88" s="7" t="s">
         <v>20</v>
@@ -6368,10 +6378,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D89" s="1">
         <v>2025</v>
@@ -6380,14 +6390,14 @@
         <v>103</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H89" s="1" t="str">
         <f>VLOOKUP(G89,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I89" s="7" t="s">
         <v>20</v>
@@ -6416,10 +6426,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D90" s="1">
         <v>2000</v>
@@ -6428,14 +6438,14 @@
         <v>103</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H90" s="1" t="str">
         <f>VLOOKUP(G90,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Speicher &amp; Performance</v>
+        <v xml:space="preserve">Speicher und Performance</v>
       </c>
       <c r="I90" s="7" t="s">
         <v>20</v>
@@ -6464,10 +6474,10 @@
         <v>90</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D91" s="1">
         <v>2024</v>
@@ -6483,7 +6493,7 @@
       </c>
       <c r="H91" s="1" t="str">
         <f>VLOOKUP(G91,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Grundlagen &amp; Theorien</v>
+        <v xml:space="preserve">Grundlagen und Theorien</v>
       </c>
       <c r="I91" s="7" t="s">
         <v>20</v>
@@ -6512,10 +6522,10 @@
         <v>91</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D92" s="1">
         <v>2000</v>
@@ -6527,11 +6537,11 @@
         <v>116</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="H92" s="1" t="str">
         <f>VLOOKUP(G92,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Hardware &amp; Logik</v>
+        <v xml:space="preserve">Hardware und Logik</v>
       </c>
       <c r="I92" s="7" t="s">
         <v>20</v>
@@ -6560,10 +6570,10 @@
         <v>92</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D93" s="1">
         <v>2024</v>
@@ -6572,14 +6582,14 @@
         <v>103</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H93" s="1" t="str">
         <f>VLOOKUP(G93,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I93" s="7" t="s">
         <v>20</v>
@@ -6608,10 +6618,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D94" s="1">
         <v>2025</v>
@@ -6620,10 +6630,10 @@
         <v>103</v>
       </c>
       <c r="F94" s="6" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H94" s="1" t="str">
         <f>VLOOKUP(G94,Cluster!B:C,2,FALSE)</f>
@@ -6656,10 +6666,10 @@
         <v>94</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D95" s="1">
         <v>2025</v>
@@ -6668,14 +6678,14 @@
         <v>103</v>
       </c>
       <c r="F95" s="6" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H95" s="1" t="str">
         <f>VLOOKUP(G95,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I95" s="7" t="s">
         <v>20</v>
@@ -6704,10 +6714,10 @@
         <v>95</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D96" s="1">
         <v>2023</v>
@@ -6716,14 +6726,14 @@
         <v>103</v>
       </c>
       <c r="F96" s="6" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H96" s="1" t="str">
         <f>VLOOKUP(G96,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I96" s="7" t="s">
         <v>20</v>
@@ -6752,10 +6762,10 @@
         <v>96</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D97" s="1">
         <v>2025</v>
@@ -6764,14 +6774,14 @@
         <v>103</v>
       </c>
       <c r="F97" s="6" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="G97" s="6" t="s">
         <v>179</v>
       </c>
       <c r="H97" s="1" t="str">
         <f>VLOOKUP(G97,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Hardware &amp; Logik</v>
+        <v xml:space="preserve">Hardware und Logik</v>
       </c>
       <c r="I97" s="7" t="s">
         <v>20</v>
@@ -6800,10 +6810,10 @@
         <v>97</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D98" s="1">
         <v>2025</v>
@@ -6812,14 +6822,14 @@
         <v>103</v>
       </c>
       <c r="F98" s="6" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H98" s="1" t="str">
         <f>VLOOKUP(G98,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I98" s="7" t="s">
         <v>20</v>
@@ -6830,8 +6840,8 @@
       <c r="K98" s="2">
         <v>1</v>
       </c>
-      <c r="L98" s="8" t="s">
-        <v>22</v>
+      <c r="L98" s="8">
+        <v>3</v>
       </c>
       <c r="M98" s="2">
         <v>2</v>
@@ -6848,10 +6858,10 @@
         <v>98</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D99" s="1">
         <v>2025</v>
@@ -6860,14 +6870,14 @@
         <v>103</v>
       </c>
       <c r="F99" s="6" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H99" s="1" t="str">
         <f>VLOOKUP(G99,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I99" s="7" t="s">
         <v>20</v>
@@ -6878,8 +6888,8 @@
       <c r="K99" s="2">
         <v>1</v>
       </c>
-      <c r="L99" s="8" t="s">
-        <v>22</v>
+      <c r="L99" s="8">
+        <v>3</v>
       </c>
       <c r="M99" s="2">
         <v>1</v>
@@ -6896,10 +6906,10 @@
         <v>99</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D100" s="1">
         <v>2024</v>
@@ -6908,14 +6918,14 @@
         <v>103</v>
       </c>
       <c r="F100" s="6" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H100" s="1" t="str">
         <f>VLOOKUP(G100,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I100" s="7" t="s">
         <v>20</v>
@@ -6944,10 +6954,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D101" s="1">
         <v>2024</v>
@@ -6963,7 +6973,7 @@
       </c>
       <c r="H101" s="1" t="str">
         <f>VLOOKUP(G101,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Hardware &amp; Logik</v>
+        <v xml:space="preserve">Hardware und Logik</v>
       </c>
       <c r="I101" s="7" t="s">
         <v>20</v>
@@ -6992,10 +7002,10 @@
         <v>101</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D102" s="1">
         <v>2019</v>
@@ -7007,11 +7017,11 @@
         <v>116</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H102" s="1" t="str">
         <f>VLOOKUP(G102,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I102" s="7" t="s">
         <v>20</v>
@@ -7022,8 +7032,8 @@
       <c r="K102" s="2">
         <v>1</v>
       </c>
-      <c r="L102" s="8" t="s">
-        <v>22</v>
+      <c r="L102" s="8">
+        <v>3</v>
       </c>
       <c r="M102" s="2">
         <v>0</v>
@@ -7040,10 +7050,10 @@
         <v>102</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D103" s="1">
         <v>2019</v>
@@ -7059,7 +7069,7 @@
       </c>
       <c r="H103" s="1" t="str">
         <f>VLOOKUP(G103,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Hardware &amp; Logik</v>
+        <v xml:space="preserve">Hardware und Logik</v>
       </c>
       <c r="I103" s="7" t="s">
         <v>20</v>
@@ -7088,10 +7098,10 @@
         <v>103</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D104" s="1">
         <v>2025</v>
@@ -7100,14 +7110,14 @@
         <v>103</v>
       </c>
       <c r="F104" s="6" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H104" s="1" t="str">
         <f>VLOOKUP(G104,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I104" s="7" t="s">
         <v>20</v>
@@ -7118,8 +7128,8 @@
       <c r="K104" s="2">
         <v>1</v>
       </c>
-      <c r="L104" s="2" t="s">
-        <v>22</v>
+      <c r="L104" s="2">
+        <v>3</v>
       </c>
       <c r="M104" s="2">
         <v>0</v>
@@ -7136,10 +7146,10 @@
         <v>104</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D105" s="1">
         <v>2022</v>
@@ -7148,14 +7158,14 @@
         <v>103</v>
       </c>
       <c r="F105" s="6" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H105" s="1" t="str">
         <f>VLOOKUP(G105,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I105" s="7" t="s">
         <v>20</v>
@@ -7184,10 +7194,10 @@
         <v>105</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D106" s="1">
         <v>2024</v>
@@ -7196,10 +7206,10 @@
         <v>103</v>
       </c>
       <c r="F106" s="6" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H106" s="1" t="str">
         <f>VLOOKUP(G106,Cluster!B:C,2,FALSE)</f>
@@ -7232,10 +7242,10 @@
         <v>106</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D107" s="1">
         <v>2022</v>
@@ -7244,14 +7254,14 @@
         <v>17</v>
       </c>
       <c r="F107" s="6" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H107" s="1" t="str">
         <f>VLOOKUP(G107,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Speicher &amp; Performance</v>
+        <v xml:space="preserve">Speicher und Performance</v>
       </c>
       <c r="I107" s="7" t="s">
         <v>20</v>
@@ -7280,10 +7290,10 @@
         <v>107</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D108" s="1">
         <v>2025</v>
@@ -7292,14 +7302,14 @@
         <v>103</v>
       </c>
       <c r="F108" s="6" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H108" s="1" t="str">
         <f>VLOOKUP(G108,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Systeme &amp; Anwendungen</v>
+        <v xml:space="preserve">Systeme und Anwendungen</v>
       </c>
       <c r="I108" s="7" t="s">
         <v>20</v>
@@ -7328,10 +7338,10 @@
         <v>108</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D109" s="1">
         <v>2024</v>
@@ -7340,14 +7350,14 @@
         <v>103</v>
       </c>
       <c r="F109" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="G109" s="6" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H109" s="1" t="str">
         <f>VLOOKUP(G109,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Systeme &amp; Anwendungen</v>
+        <v xml:space="preserve">Systeme und Anwendungen</v>
       </c>
       <c r="I109" s="7" t="s">
         <v>21</v>
@@ -7376,10 +7386,10 @@
         <v>109</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D110" s="1">
         <v>2024</v>
@@ -7388,10 +7398,10 @@
         <v>103</v>
       </c>
       <c r="F110" s="6" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H110" s="1" t="str">
         <f>VLOOKUP(G110,Cluster!B:C,2,FALSE)</f>
@@ -7424,10 +7434,10 @@
         <v>110</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D111" s="1">
         <v>2024</v>
@@ -7443,7 +7453,7 @@
       </c>
       <c r="H111" s="1" t="str">
         <f>VLOOKUP(G111,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Grundlagen &amp; Theorien</v>
+        <v xml:space="preserve">Grundlagen und Theorien</v>
       </c>
       <c r="I111" s="7" t="s">
         <v>20</v>
@@ -7472,10 +7482,10 @@
         <v>111</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D112" s="1">
         <v>2024</v>
@@ -7484,14 +7494,14 @@
         <v>103</v>
       </c>
       <c r="F112" s="6" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H112" s="1" t="str">
         <f>VLOOKUP(G112,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Systeme &amp; Anwendungen</v>
+        <v xml:space="preserve">Systeme und Anwendungen</v>
       </c>
       <c r="I112" s="7" t="s">
         <v>20</v>
@@ -7520,10 +7530,10 @@
         <v>112</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D113" s="1">
         <v>2024</v>
@@ -7532,10 +7542,10 @@
         <v>103</v>
       </c>
       <c r="F113" s="6" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H113" s="1" t="str">
         <f>VLOOKUP(G113,Cluster!B:C,2,FALSE)</f>
@@ -7568,10 +7578,10 @@
         <v>113</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D114" s="1">
         <v>2025</v>
@@ -7580,14 +7590,14 @@
         <v>103</v>
       </c>
       <c r="F114" s="6" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="H114" s="1" t="str">
         <f>VLOOKUP(G114,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Systeme &amp; Anwendungen</v>
+        <v xml:space="preserve">Systeme und Anwendungen</v>
       </c>
       <c r="I114" s="7" t="s">
         <v>20</v>
@@ -7596,7 +7606,7 @@
         <v>20</v>
       </c>
       <c r="K114" s="7" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="L114" s="2">
         <v>1</v>
@@ -7616,10 +7626,10 @@
         <v>114</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D115" s="1">
         <v>2025</v>
@@ -7631,7 +7641,7 @@
         <v>144</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H115" s="1" t="str">
         <f>VLOOKUP(G115,Cluster!B:C,2,FALSE)</f>
@@ -7664,10 +7674,10 @@
         <v>115</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D116" s="1">
         <v>2015</v>
@@ -7676,14 +7686,14 @@
         <v>103</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H116" s="1" t="str">
         <f>VLOOKUP(G116,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I116" s="7" t="s">
         <v>20</v>
@@ -7712,10 +7722,10 @@
         <v>116</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D117" s="1">
         <v>2023</v>
@@ -7724,7 +7734,7 @@
         <v>103</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="G117" s="6" t="s">
         <v>210</v>
@@ -7760,10 +7770,10 @@
         <v>117</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D118" s="1">
         <v>2023</v>
@@ -7772,14 +7782,14 @@
         <v>103</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="G118" s="6" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="H118" s="1" t="str">
         <f>VLOOKUP(G118,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Grundlagen &amp; Theorien</v>
+        <v xml:space="preserve">Grundlagen und Theorien</v>
       </c>
       <c r="I118" s="7" t="s">
         <v>20</v>
@@ -7808,10 +7818,10 @@
         <v>118</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D119" s="1">
         <v>2025</v>
@@ -7820,14 +7830,14 @@
         <v>103</v>
       </c>
       <c r="F119" s="6" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="G119" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H119" s="1" t="str">
         <f>VLOOKUP(G119,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Speicher &amp; Performance</v>
+        <v xml:space="preserve">Speicher und Performance</v>
       </c>
       <c r="I119" s="7" t="s">
         <v>20</v>
@@ -7856,10 +7866,10 @@
         <v>119</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D120" s="1">
         <v>2025</v>
@@ -7868,14 +7878,14 @@
         <v>17</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H120" s="1" t="str">
         <f>VLOOKUP(G120,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Systeme &amp; Anwendungen</v>
+        <v xml:space="preserve">Systeme und Anwendungen</v>
       </c>
       <c r="I120" s="7" t="s">
         <v>20</v>
@@ -7904,10 +7914,10 @@
         <v>120</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D121" s="1">
         <v>2025</v>
@@ -7916,14 +7926,14 @@
         <v>103</v>
       </c>
       <c r="F121" s="6" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="H121" s="1" t="str">
         <f>VLOOKUP(G121,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I121" s="7" t="s">
         <v>20</v>
@@ -7952,10 +7962,10 @@
         <v>121</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D122" s="1">
         <v>2024</v>
@@ -7964,7 +7974,7 @@
         <v>103</v>
       </c>
       <c r="F122" s="6" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="G122" s="6" t="s">
         <v>210</v>
@@ -8000,10 +8010,10 @@
         <v>122</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D123" s="1">
         <v>2020</v>
@@ -8012,14 +8022,14 @@
         <v>103</v>
       </c>
       <c r="F123" s="6" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="G123" s="6" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H123" s="1" t="str">
         <f>VLOOKUP(G123,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Systeme &amp; Anwendungen</v>
+        <v xml:space="preserve">Systeme und Anwendungen</v>
       </c>
       <c r="I123" s="7" t="s">
         <v>20</v>
@@ -8048,10 +8058,10 @@
         <v>123</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D124" s="1">
         <v>2023</v>
@@ -8060,14 +8070,14 @@
         <v>17</v>
       </c>
       <c r="F124" s="6" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="G124" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H124" s="1" t="str">
         <f>VLOOKUP(G124,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Speicher &amp; Performance</v>
+        <v xml:space="preserve">Speicher und Performance</v>
       </c>
       <c r="I124" s="7" t="s">
         <v>20</v>
@@ -8096,10 +8106,10 @@
         <v>124</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D125" s="1">
         <v>1999</v>
@@ -8108,14 +8118,14 @@
         <v>17</v>
       </c>
       <c r="F125" s="6" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="G125" s="6" t="s">
         <v>153</v>
       </c>
       <c r="H125" s="1" t="str">
         <f>VLOOKUP(G125,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I125" s="7" t="s">
         <v>20</v>
@@ -8144,10 +8154,10 @@
         <v>125</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D126" s="1">
         <v>2005</v>
@@ -8156,14 +8166,14 @@
         <v>17</v>
       </c>
       <c r="F126" s="6" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="G126" s="6" t="s">
         <v>153</v>
       </c>
       <c r="H126" s="1" t="str">
         <f>VLOOKUP(G126,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I126" s="7" t="s">
         <v>20</v>
@@ -8174,8 +8184,8 @@
       <c r="K126" s="2">
         <v>1</v>
       </c>
-      <c r="L126" s="8" t="s">
-        <v>22</v>
+      <c r="L126" s="8">
+        <v>3</v>
       </c>
       <c r="M126" s="2">
         <v>0</v>
@@ -8192,10 +8202,10 @@
         <v>126</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D127" s="1">
         <v>2004</v>
@@ -8207,11 +8217,11 @@
         <v>116</v>
       </c>
       <c r="G127" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H127" s="1" t="str">
         <f>VLOOKUP(G127,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I127" s="7" t="s">
         <v>20</v>
@@ -8240,10 +8250,10 @@
         <v>127</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D128" s="1">
         <v>2009</v>
@@ -8252,14 +8262,14 @@
         <v>17</v>
       </c>
       <c r="F128" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G128" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H128" s="1" t="str">
         <f>VLOOKUP(G128,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I128" s="7" t="s">
         <v>20</v>
@@ -8288,10 +8298,10 @@
         <v>128</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D129" s="1">
         <v>1990</v>
@@ -8300,7 +8310,7 @@
         <v>17</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G129" s="1" t="s">
         <v>19</v>
@@ -8336,10 +8346,10 @@
         <v>129</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D130" s="1">
         <v>2017</v>
@@ -8348,14 +8358,14 @@
         <v>103</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H130" s="1" t="str">
         <f>VLOOKUP(G130,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I130" s="2">
         <v>0</v>
@@ -8384,10 +8394,10 @@
         <v>130</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D131" s="1">
         <v>2012</v>
@@ -8396,14 +8406,14 @@
         <v>17</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H131" s="1" t="str">
         <f>VLOOKUP(G131,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I131" s="2">
         <v>0</v>
@@ -8432,10 +8442,10 @@
         <v>131</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D132" s="1">
         <v>2013</v>
@@ -8444,7 +8454,7 @@
         <v>17</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="G132" s="1" t="s">
         <v>19</v>
@@ -8462,8 +8472,8 @@
       <c r="K132" s="2">
         <v>1</v>
       </c>
-      <c r="L132" s="8" t="s">
-        <v>22</v>
+      <c r="L132" s="8">
+        <v>3</v>
       </c>
       <c r="M132" s="2">
         <v>0</v>
@@ -8483,7 +8493,7 @@
         <v>163</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D133" s="1">
         <v>2013</v>
@@ -8492,14 +8502,14 @@
         <v>17</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="G133" s="1" t="s">
         <v>196</v>
       </c>
       <c r="H133" s="1" t="str">
         <f>VLOOKUP(G133,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Grundlagen &amp; Theorien</v>
+        <v xml:space="preserve">Grundlagen und Theorien</v>
       </c>
       <c r="I133" s="2">
         <v>0</v>
@@ -8528,10 +8538,10 @@
         <v>133</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D134" s="1">
         <v>2016</v>
@@ -8540,14 +8550,14 @@
         <v>17</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H134" s="1" t="str">
         <f>VLOOKUP(G134,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I134" s="2">
         <v>0</v>
@@ -8576,10 +8586,10 @@
         <v>134</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D135" s="1">
         <v>1999</v>
@@ -8588,14 +8598,14 @@
         <v>17</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H135" s="1" t="str">
         <f>VLOOKUP(G135,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I135" s="2">
         <v>0</v>
@@ -8624,10 +8634,10 @@
         <v>135</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D136" s="1">
         <v>2003</v>
@@ -8636,14 +8646,14 @@
         <v>103</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="G136" s="1" t="s">
         <v>179</v>
       </c>
       <c r="H136" s="1" t="str">
         <f>VLOOKUP(G136,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Hardware &amp; Logik</v>
+        <v xml:space="preserve">Hardware und Logik</v>
       </c>
       <c r="I136" s="2">
         <v>0</v>
@@ -8672,10 +8682,10 @@
         <v>136</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D137" s="1">
         <v>2012</v>
@@ -8684,14 +8694,14 @@
         <v>103</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H137" s="1" t="str">
         <f>VLOOKUP(G137,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I137" s="2">
         <v>0</v>
@@ -8720,10 +8730,10 @@
         <v>137</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D138" s="1">
         <v>2004</v>
@@ -8732,14 +8742,14 @@
         <v>103</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="G138" s="1" t="s">
         <v>207</v>
       </c>
       <c r="H138" s="1" t="str">
         <f>VLOOKUP(G138,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Hardware &amp; Logik</v>
+        <v xml:space="preserve">Hardware und Logik</v>
       </c>
       <c r="I138" s="2">
         <v>0</v>
@@ -8768,10 +8778,10 @@
         <v>138</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D139" s="1">
         <v>2000</v>
@@ -8780,7 +8790,7 @@
         <v>103</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="G139" s="1" t="s">
         <v>19</v>
@@ -8816,10 +8826,10 @@
         <v>139</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D140" s="1">
         <v>2008</v>
@@ -8828,14 +8838,14 @@
         <v>17</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="G140" s="1" t="s">
         <v>196</v>
       </c>
       <c r="H140" s="1" t="str">
         <f>VLOOKUP(G140,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Grundlagen &amp; Theorien</v>
+        <v xml:space="preserve">Grundlagen und Theorien</v>
       </c>
       <c r="I140" s="2">
         <v>0</v>
@@ -8864,22 +8874,26 @@
         <v>140</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D141" s="1">
         <v>2013</v>
       </c>
-      <c r="E141" s="1"/>
-      <c r="F141" s="1"/>
+      <c r="E141" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="G141" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H141" s="1" t="str">
         <f>VLOOKUP(G141,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Speicher &amp; Performance</v>
+        <v xml:space="preserve">Speicher und Performance</v>
       </c>
       <c r="I141" s="2">
         <v>0</v>
@@ -8908,10 +8922,10 @@
         <v>141</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D142" s="1">
         <v>2020</v>
@@ -8920,14 +8934,14 @@
         <v>257</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="G142" s="1" t="s">
         <v>196</v>
       </c>
       <c r="H142" s="1" t="str">
         <f>VLOOKUP(G142,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Grundlagen &amp; Theorien</v>
+        <v xml:space="preserve">Grundlagen und Theorien</v>
       </c>
       <c r="I142" s="2">
         <v>1</v>
@@ -8956,10 +8970,10 @@
         <v>142</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="D143" s="1">
         <v>1995</v>
@@ -8968,14 +8982,14 @@
         <v>103</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H143" s="1" t="str">
         <f>VLOOKUP(G143,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Speicher &amp; Performance</v>
+        <v xml:space="preserve">Speicher und Performance</v>
       </c>
       <c r="I143" s="2">
         <v>0</v>
@@ -9004,10 +9018,10 @@
         <v>143</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="D144" s="1">
         <v>2003</v>
@@ -9019,11 +9033,11 @@
         <v>134</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H144" s="1" t="str">
         <f>VLOOKUP(G144,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I144" s="2">
         <v>1</v>
@@ -9052,10 +9066,10 @@
         <v>144</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D145" s="1">
         <v>2003</v>
@@ -9064,14 +9078,14 @@
         <v>17</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H145" s="1" t="str">
         <f>VLOOKUP(G145,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I145" s="2">
         <v>1</v>
@@ -9100,10 +9114,10 @@
         <v>145</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="D146" s="1">
         <v>2003</v>
@@ -9115,11 +9129,11 @@
         <v>122</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H146" s="1" t="str">
         <f>VLOOKUP(G146,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Speicher &amp; Performance</v>
+        <v xml:space="preserve">Speicher und Performance</v>
       </c>
       <c r="I146" s="2">
         <v>0</v>
@@ -9148,10 +9162,10 @@
         <v>146</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="D147" s="1">
         <v>2007</v>
@@ -9160,14 +9174,14 @@
         <v>103</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="G147" s="1" t="s">
         <v>196</v>
       </c>
       <c r="H147" s="1" t="str">
         <f>VLOOKUP(G147,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Grundlagen &amp; Theorien</v>
+        <v xml:space="preserve">Grundlagen und Theorien</v>
       </c>
       <c r="I147" s="2">
         <v>1</v>
@@ -9196,10 +9210,10 @@
         <v>147</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="D148" s="1">
         <v>2007</v>
@@ -9208,14 +9222,14 @@
         <v>17</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="G148" s="1" t="s">
         <v>179</v>
       </c>
       <c r="H148" s="1" t="str">
         <f>VLOOKUP(G148,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Hardware &amp; Logik</v>
+        <v xml:space="preserve">Hardware und Logik</v>
       </c>
       <c r="I148" s="2">
         <v>0</v>
@@ -9244,10 +9258,10 @@
         <v>148</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="D149" s="1">
         <v>2002</v>
@@ -9256,14 +9270,14 @@
         <v>103</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H149" s="1" t="str">
         <f>VLOOKUP(G149,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I149" s="2">
         <v>0</v>
@@ -9292,10 +9306,10 @@
         <v>149</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="D150" s="1">
         <v>2025</v>
@@ -9304,14 +9318,14 @@
         <v>103</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H150" s="1" t="str">
         <f>VLOOKUP(G150,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I150" s="2">
         <v>0</v>
@@ -9340,10 +9354,10 @@
         <v>150</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="D151" s="1">
         <v>2025</v>
@@ -9352,14 +9366,14 @@
         <v>103</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H151" s="1" t="str">
         <f>VLOOKUP(G151,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Prozessoren &amp; Architekturen</v>
+        <v xml:space="preserve">Prozessoren und Architekturen</v>
       </c>
       <c r="I151" s="2">
         <v>0</v>
@@ -9388,10 +9402,10 @@
         <v>151</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="D152" s="1">
         <v>2023</v>
@@ -9400,14 +9414,14 @@
         <v>103</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="G152" s="1" t="s">
         <v>179</v>
       </c>
       <c r="H152" s="1" t="str">
         <f>VLOOKUP(G152,Cluster!B:C,2,FALSE)</f>
-        <v xml:space="preserve">Hardware &amp; Logik</v>
+        <v xml:space="preserve">Hardware und Logik</v>
       </c>
       <c r="I152" s="2">
         <v>0</v>
@@ -9470,7 +9484,7 @@
       <c r="A164" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O1"/>
+  <autoFilter ref="A1:O152"/>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup paperSize="9" scale="72" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
@@ -9500,7 +9514,7 @@
   <sheetData>
     <row r="2">
       <c r="B2" s="11" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="C2" s="12">
         <v>0</v>
@@ -9512,7 +9526,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -9520,10 +9534,10 @@
         <v>9</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
     </row>
     <row r="4">
@@ -9531,16 +9545,16 @@
         <v>10</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="5" ht="12.75">
@@ -9548,10 +9562,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
     </row>
     <row r="6" ht="12.75">
@@ -9559,13 +9573,16 @@
         <v>11</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>457</v>
+        <v>459</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="7" ht="12.75">
@@ -9573,13 +9590,13 @@
         <v>12</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="D7" s="10" t="s">
+        <v>462</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>459</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="8" ht="12.75">
@@ -9587,13 +9604,13 @@
         <v>13</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -9624,7 +9641,7 @@
     </row>
     <row r="3" ht="12.75">
       <c r="B3" s="10" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>7</v>
@@ -9632,10 +9649,10 @@
     </row>
     <row r="4" ht="12.75">
       <c r="B4" s="10" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="5" ht="12.75">
@@ -9643,7 +9660,7 @@
         <v>196</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="6" ht="12.75">
@@ -9651,15 +9668,15 @@
         <v>128</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="7" ht="12.75">
       <c r="B7" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="8" ht="12.75">
@@ -9667,39 +9684,39 @@
         <v>185</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="9" ht="12.75">
       <c r="B9" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="10" ht="12.75">
       <c r="B10" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="11" ht="12.75">
       <c r="B11" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="12" ht="12.75">
       <c r="B12" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="13" ht="12.75">
@@ -9707,63 +9724,63 @@
         <v>153</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="14" ht="12.75">
       <c r="B14" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="15" ht="12.75">
       <c r="B15" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="16" ht="12.75">
       <c r="B16" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="17" ht="12.75">
       <c r="B17" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="18" ht="12.75">
       <c r="B18" s="10" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="19" ht="12.75">
       <c r="B19" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
     </row>
     <row r="20" ht="12.75">
       <c r="B20" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
     </row>
     <row r="21" ht="12.75">
@@ -9771,7 +9788,7 @@
         <v>203</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
     </row>
     <row r="22" ht="12.75">
@@ -9779,7 +9796,7 @@
         <v>145</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
     </row>
     <row r="23" ht="12.75">
@@ -9787,7 +9804,7 @@
         <v>225</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="24" ht="12.75">
@@ -9795,7 +9812,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
     </row>
     <row r="25" ht="12.75">
@@ -9803,15 +9820,15 @@
         <v>207</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="26" ht="12.75">
       <c r="B26" s="10" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="27" ht="12.75">
@@ -9819,31 +9836,31 @@
         <v>179</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="28" ht="12.75">
       <c r="B28" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="29" ht="12.75">
       <c r="B29" s="10" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
     </row>
     <row r="30" ht="12.75">
       <c r="B30" s="10" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="31" ht="12.75">
@@ -9851,15 +9868,15 @@
         <v>200</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="32" ht="12.75">
       <c r="B32" s="10" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="33" ht="12.75">
@@ -9880,10 +9897,10 @@
     </row>
     <row r="35" ht="12.75">
       <c r="B35" s="10" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="41" ht="12.75">

</xml_diff>